<commit_message>
Add missing iso's to RCP mapping file
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/RCP/RCP Region Mapping.xlsx
+++ b/input/emissions-inventories/RCP/RCP Region Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="320" windowWidth="20860" windowHeight="14120" tabRatio="657"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="657" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reg Codes" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="708">
   <si>
     <t>Check</t>
   </si>
@@ -2510,13 +2510,64 @@
   </si>
   <si>
     <t>BFA</t>
+  </si>
+  <si>
+    <t>cuw</t>
+  </si>
+  <si>
+    <t>mne</t>
+  </si>
+  <si>
+    <t>pse</t>
+  </si>
+  <si>
+    <t>rou</t>
+  </si>
+  <si>
+    <t>srb</t>
+  </si>
+  <si>
+    <t>srb (kosovo)</t>
+  </si>
+  <si>
+    <t>ssd</t>
+  </si>
+  <si>
+    <t>sxm</t>
+  </si>
+  <si>
+    <t>tls</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Other S. &amp; Cent. America</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times"/>
@@ -2541,10 +2592,6 @@
       <name val="Times"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Times"/>
@@ -2553,6 +2600,18 @@
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Times"/>
     </font>
   </fonts>
@@ -2606,9 +2665,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2639,7 +2724,33 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="28">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_CrudeOil_IEACountries" xfId="1"/>
   </cellStyles>
@@ -3022,7 +3133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5693,7 +5804,7 @@
         <v>132</v>
       </c>
       <c r="F98" t="b">
-        <f t="shared" ref="F98:F129" si="3">E98=B98</f>
+        <f t="shared" ref="F98:F100" si="3">E98=B98</f>
         <v>1</v>
       </c>
       <c r="H98" s="10" t="s">
@@ -6645,13 +6756,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H235"/>
+  <dimension ref="A1:H244"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C204" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C220" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G213" sqref="G213"/>
+      <selection pane="bottomRight" activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -11359,10 +11470,187 @@
         <v>608</v>
       </c>
     </row>
+    <row r="236" spans="1:8">
+      <c r="A236" t="s">
+        <v>691</v>
+      </c>
+      <c r="B236" t="s">
+        <v>700</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D236" s="6">
+        <v>24</v>
+      </c>
+      <c r="F236" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H236" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8">
+      <c r="A237" t="s">
+        <v>692</v>
+      </c>
+      <c r="B237" t="s">
+        <v>701</v>
+      </c>
+      <c r="C237" t="s">
+        <v>375</v>
+      </c>
+      <c r="D237">
+        <v>33</v>
+      </c>
+      <c r="F237" t="s">
+        <v>375</v>
+      </c>
+      <c r="H237" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8">
+      <c r="A238" t="s">
+        <v>693</v>
+      </c>
+      <c r="B238" t="s">
+        <v>702</v>
+      </c>
+      <c r="D238">
+        <v>18</v>
+      </c>
+      <c r="F238" t="s">
+        <v>413</v>
+      </c>
+      <c r="H238" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8">
+      <c r="A239" t="s">
+        <v>694</v>
+      </c>
+      <c r="B239" t="s">
+        <v>496</v>
+      </c>
+      <c r="C239" t="s">
+        <v>374</v>
+      </c>
+      <c r="D239">
+        <v>33</v>
+      </c>
+      <c r="F239" t="s">
+        <v>374</v>
+      </c>
+      <c r="H239" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8">
+      <c r="A240" t="s">
+        <v>695</v>
+      </c>
+      <c r="B240" t="s">
+        <v>703</v>
+      </c>
+      <c r="C240" t="s">
+        <v>375</v>
+      </c>
+      <c r="D240">
+        <v>33</v>
+      </c>
+      <c r="F240" t="s">
+        <v>375</v>
+      </c>
+      <c r="H240" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8">
+      <c r="A241" t="s">
+        <v>696</v>
+      </c>
+      <c r="B241" t="s">
+        <v>704</v>
+      </c>
+      <c r="C241" t="s">
+        <v>375</v>
+      </c>
+      <c r="D241">
+        <v>33</v>
+      </c>
+      <c r="F241" t="s">
+        <v>375</v>
+      </c>
+      <c r="H241" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8">
+      <c r="A242" t="s">
+        <v>697</v>
+      </c>
+      <c r="B242" t="s">
+        <v>705</v>
+      </c>
+      <c r="C242" t="s">
+        <v>76</v>
+      </c>
+      <c r="D242">
+        <v>21</v>
+      </c>
+      <c r="F242" t="s">
+        <v>76</v>
+      </c>
+      <c r="H242" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8">
+      <c r="A243" t="s">
+        <v>698</v>
+      </c>
+      <c r="B243" t="s">
+        <v>706</v>
+      </c>
+      <c r="C243" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D243" s="6">
+        <v>24</v>
+      </c>
+      <c r="F243" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H243" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8">
+      <c r="A244" t="s">
+        <v>699</v>
+      </c>
+      <c r="B244" t="s">
+        <v>707</v>
+      </c>
+      <c r="C244" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D244" s="6">
+        <v>32</v>
+      </c>
+      <c r="F244" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="H244" t="s">
+        <v>612</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>